<commit_message>
Dodane sprawozdanie z semestru
</commit_message>
<xml_diff>
--- a/PSI_01/Excel_01_Throw.xlsx
+++ b/PSI_01/Excel_01_Throw.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -151,14 +151,14 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3226,11 +3226,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119090176"/>
-        <c:axId val="119120640"/>
+        <c:axId val="102004224"/>
+        <c:axId val="102005760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119090176"/>
+        <c:axId val="102004224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3239,7 +3239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119120640"/>
+        <c:crossAx val="102005760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3247,7 +3247,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119120640"/>
+        <c:axId val="102005760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3258,7 +3258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119090176"/>
+        <c:crossAx val="102004224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3306,12 +3306,22 @@
           <c:order val="0"/>
           <c:invertIfNegative val="0"/>
           <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="3"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -3375,20 +3385,44 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="83605376"/>
-        <c:axId val="83606912"/>
+        <c:axId val="102038912"/>
+        <c:axId val="102831616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83605376"/>
+        <c:axId val="102038912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Numer</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> proby</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83606912"/>
+        <c:crossAx val="102831616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3396,7 +3430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83606912"/>
+        <c:axId val="102831616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3407,7 +3441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83605376"/>
+        <c:crossAx val="102038912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3793,7 +3827,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3910,27 +3946,27 @@
       <c r="A21">
         <v>346.86406666666602</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>334.20806666666601</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3938,17 +3974,17 @@
       <c r="A23">
         <v>340.50666666666598</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>4530</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>5000</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <f>C23/D23*100</f>
         <v>90.600000000000009</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>215.52019999999999</v>
       </c>
     </row>
@@ -3956,17 +3992,17 @@
       <c r="A24">
         <v>338.4006</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>4480</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>5000</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <f>C24/D24*100</f>
         <v>89.600000000000009</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>208.38820000000001</v>
       </c>
     </row>
@@ -3974,17 +4010,17 @@
       <c r="A25">
         <v>334.50666666666598</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>4503</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>5000</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <f t="shared" ref="E25:E32" si="0">C25/D25*100</f>
         <v>90.06</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>209.80500000000001</v>
       </c>
     </row>
@@ -3992,17 +4028,17 @@
       <c r="A26">
         <v>326.78640000000001</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>4506</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>5000</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <f t="shared" si="0"/>
         <v>90.12</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>216.96100000000001</v>
       </c>
     </row>
@@ -4010,17 +4046,17 @@
       <c r="A27">
         <v>320.32426666666601</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>4500</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>5000</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="1">
         <v>214.5624</v>
       </c>
     </row>
@@ -4028,17 +4064,17 @@
       <c r="A28">
         <v>326.49126666666598</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>4026</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>5000</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <f t="shared" si="0"/>
         <v>80.52</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="1">
         <v>213.12960000000001</v>
       </c>
     </row>
@@ -4046,17 +4082,17 @@
       <c r="A29">
         <v>315.08506666666602</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>4505</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>5000</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <f t="shared" si="0"/>
         <v>90.100000000000009</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="1">
         <v>219.857</v>
       </c>
     </row>
@@ -4064,17 +4100,17 @@
       <c r="A30">
         <v>314.50560000000002</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>4471</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>5000</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <f t="shared" si="0"/>
         <v>89.42</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>215.041</v>
       </c>
     </row>
@@ -4082,17 +4118,17 @@
       <c r="A31">
         <v>309.889066666666</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>4446</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>5000</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="1">
         <f t="shared" si="0"/>
         <v>88.92</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="1">
         <v>211.22659999999999</v>
       </c>
     </row>
@@ -4100,17 +4136,17 @@
       <c r="A32">
         <v>303.88166666666598</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>4491</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>5000</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <f t="shared" si="0"/>
         <v>89.82</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="3">
         <v>207.44640000000001</v>
       </c>
     </row>

</xml_diff>